<commit_message>
Fixed numerous issues, saving presets path to user config, added K!!!
</commit_message>
<xml_diff>
--- a/Resources/FilamentPresets.xlsx
+++ b/Resources/FilamentPresets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\BambuUserFilamentGenerator\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E9FEA7-CB23-4F9F-A9F7-468FD4570E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA478AFE-8A51-47DB-9967-1E4A95B8EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5719292B-9672-4C9F-9E29-C5454A8C8A2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{5719292B-9672-4C9F-9E29-C5454A8C8A2A}"/>
   </bookViews>
   <sheets>
     <sheet name="PLA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>Brand</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>NEO Base</t>
+  </si>
+  <si>
+    <t>Yellow</t>
   </si>
 </sst>
 </file>
@@ -492,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E73D34-F7F0-4F5F-95F0-637D7D21B460}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,16 +865,36 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1">
+        <v>190</v>
+      </c>
+      <c r="F12" s="1">
+        <v>220</v>
+      </c>
+      <c r="G12" s="1">
+        <v>220</v>
+      </c>
+      <c r="H12" s="1">
+        <v>220</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="J12" s="1">
+        <v>3.2000000000000001E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -1098,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A91E9F8-6BE0-4465-932A-36C9781C3E51}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>

</xml_diff>